<commit_message>
damn type checking is ugly code!
</commit_message>
<xml_diff>
--- a/PMConverter/src/test.xlsx
+++ b/PMConverter/src/test.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
   <si>
     <t>General</t>
   </si>
@@ -78,10 +78,22 @@
     <t>(1,)</t>
   </si>
   <si>
-    <t>[()]</t>
+    <t>[]</t>
+  </si>
+  <si>
+    <t>[(&lt;object.Activity.Activity object at 0x7f5311b13ef0&gt;, 'FS', 0)]</t>
   </si>
   <si>
     <t>0</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>(1, 1)</t>
+  </si>
+  <si>
+    <t>[(&lt;object.Activity.Activity object at 0x7f5311b13eb8&gt;, 'FS', 0)]</t>
   </si>
 </sst>
 </file>
@@ -422,7 +434,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -522,19 +534,19 @@
         <v>20</v>
       </c>
       <c r="E3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F3">
-        <v>42097.5100302132</v>
+        <v>42097.6407448236</v>
       </c>
       <c r="G3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H3">
-        <v>42102.5100302133</v>
+        <v>42102.6407448236</v>
       </c>
       <c r="I3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J3">
         <v>0</v>
@@ -549,6 +561,50 @@
         <v>1000</v>
       </c>
       <c r="N3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4">
+        <v>42097.6407448238</v>
+      </c>
+      <c r="G4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4">
+        <v>42107.6407448238</v>
+      </c>
+      <c r="I4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>10000</v>
+      </c>
+      <c r="L4">
+        <v>10000</v>
+      </c>
+      <c r="M4">
+        <v>10000</v>
+      </c>
+      <c r="N4">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Reading + writing of baseline schedule sheet
</commit_message>
<xml_diff>
--- a/PMConverter/src/test.xlsx
+++ b/PMConverter/src/test.xlsx
@@ -81,7 +81,7 @@
     <t>[]</t>
   </si>
   <si>
-    <t>[(&lt;object.Activity.Activity object at 0x7f6329a0bf28&gt;, 'FS', 0)]</t>
+    <t>[(2, 'FS', 0)]</t>
   </si>
   <si>
     <t>0</t>
@@ -93,7 +93,7 @@
     <t>(1, 1)</t>
   </si>
   <si>
-    <t>[(&lt;object.Activity.Activity object at 0x7f6329a0bef0&gt;, 'FS', 0)]</t>
+    <t>[(1, 'FS', 0)]</t>
   </si>
 </sst>
 </file>
@@ -537,13 +537,13 @@
         <v>21</v>
       </c>
       <c r="F3">
-        <v>42101.4772053639</v>
+        <v>42103.5082590986</v>
       </c>
       <c r="G3" t="s">
         <v>22</v>
       </c>
       <c r="H3">
-        <v>42106.477205364</v>
+        <v>42108.5082590988</v>
       </c>
       <c r="I3" t="s">
         <v>22</v>
@@ -581,13 +581,13 @@
         <v>20</v>
       </c>
       <c r="F4">
-        <v>42101.4772053641</v>
+        <v>42103.5082590989</v>
       </c>
       <c r="G4" t="s">
         <v>22</v>
       </c>
       <c r="H4">
-        <v>42111.4772053641</v>
+        <v>42113.508259099</v>
       </c>
       <c r="I4" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
writing xlsx parser + adding activity
</commit_message>
<xml_diff>
--- a/PMConverter/src/test.xlsx
+++ b/PMConverter/src/test.xlsx
@@ -75,7 +75,7 @@
     <t>App Dev</t>
   </si>
   <si>
-    <t>(1,)</t>
+    <t>1.</t>
   </si>
   <si>
     <t>[]</t>
@@ -90,7 +90,7 @@
     <t>Testing</t>
   </si>
   <si>
-    <t>(1, 1)</t>
+    <t>1.1.</t>
   </si>
   <si>
     <t>[(1, 'FS', 0)]</t>
@@ -111,18 +111,36 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0000FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -137,9 +155,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -443,7 +469,7 @@
     <col min="1" max="1" width="3.7109375" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" customWidth="1"/>
     <col min="3" max="3" width="8.7109375" customWidth="1"/>
-    <col min="4" max="7" width="12.7109375" customWidth="1"/>
+    <col min="4" max="7" width="14.7109375" customWidth="1"/>
     <col min="8" max="8" width="8.7109375" customWidth="1"/>
     <col min="9" max="9" width="25.7109375" customWidth="1"/>
     <col min="10" max="10" width="10.7109375" customWidth="1"/>
@@ -476,7 +502,7 @@
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" ht="30" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -521,90 +547,90 @@
       </c>
     </row>
     <row r="3" spans="1:14">
-      <c r="A3">
+      <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="F3">
-        <v>42103.5082590986</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="F3" s="3">
+        <v>42108.6348850162</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H3">
-        <v>42108.5082590988</v>
-      </c>
-      <c r="I3" t="s">
+      <c r="H3" s="3">
+        <v>42113.6348850164</v>
+      </c>
+      <c r="I3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="J3">
+      <c r="J3" s="3">
         <v>0</v>
       </c>
-      <c r="K3">
+      <c r="K3" s="3">
         <v>1000</v>
       </c>
-      <c r="L3">
+      <c r="L3" s="3">
+        <v>0</v>
+      </c>
+      <c r="M3" s="3">
         <v>1000</v>
       </c>
-      <c r="M3">
-        <v>1000</v>
-      </c>
-      <c r="N3">
+      <c r="N3" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:14">
-      <c r="A4">
+      <c r="A4" s="2">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F4">
-        <v>42103.5082590989</v>
-      </c>
-      <c r="G4" t="s">
+      <c r="F4" s="3">
+        <v>42108.6348850165</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H4">
-        <v>42113.508259099</v>
-      </c>
-      <c r="I4" t="s">
+      <c r="H4" s="3">
+        <v>42118.6348850166</v>
+      </c>
+      <c r="I4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="J4">
+      <c r="J4" s="3">
         <v>0</v>
       </c>
-      <c r="K4">
+      <c r="K4" s="3">
         <v>10000</v>
       </c>
-      <c r="L4">
-        <v>10000</v>
-      </c>
-      <c r="M4">
-        <v>10000</v>
-      </c>
-      <c r="N4">
+      <c r="L4" s="3">
+        <v>10</v>
+      </c>
+      <c r="M4" s="3">
+        <v>100</v>
+      </c>
+      <c r="N4" s="3">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Haven't even pushed yet today o.O
</commit_message>
<xml_diff>
--- a/PMConverter/src/test.xlsx
+++ b/PMConverter/src/test.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
     <t>General</t>
   </si>
@@ -75,32 +75,42 @@
     <t>App Dev</t>
   </si>
   <si>
-    <t>1.</t>
-  </si>
-  <si>
-    <t>[]</t>
-  </si>
-  <si>
-    <t>[(2, 'FS', 0)]</t>
-  </si>
-  <si>
-    <t>0</t>
+    <t>1</t>
+  </si>
+  <si>
+    <t>FS2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5d </t>
+  </si>
+  <si>
+    <t>Programmer [10.0 #]; Tester [5.0 #]</t>
   </si>
   <si>
     <t>Testing</t>
   </si>
   <si>
-    <t>1.1.</t>
-  </si>
-  <si>
-    <t>[(1, 'FS', 0)]</t>
+    <t>1.1</t>
+  </si>
+  <si>
+    <t>FS1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10d </t>
+  </si>
+  <si>
+    <t>Tester [50.0 #]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="mm/dd/yyyy H:MM"/>
+    <numFmt numFmtId="165" formatCode="#,##0.00 €"/>
+  </numFmts>
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -110,8 +120,15 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="8"/>
       <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -143,7 +160,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -151,19 +168,40 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -467,13 +505,15 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3.7109375" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" customWidth="1"/>
-    <col min="4" max="7" width="14.7109375" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" customWidth="1"/>
+    <col min="3" max="3" width="5.7109375" customWidth="1"/>
+    <col min="4" max="5" width="16.7109375" customWidth="1"/>
+    <col min="6" max="7" width="12.7109375" customWidth="1"/>
     <col min="8" max="8" width="8.7109375" customWidth="1"/>
     <col min="9" max="9" width="25.7109375" customWidth="1"/>
     <col min="10" max="10" width="10.7109375" customWidth="1"/>
     <col min="11" max="12" width="15.7109375" customWidth="1"/>
+    <col min="14" max="14" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -556,37 +596,35 @@
       <c r="C3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="3"/>
+      <c r="E3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="F3" s="4">
+        <v>42108.849430161</v>
+      </c>
+      <c r="G3" s="4">
+        <v>42113.8494301611</v>
+      </c>
+      <c r="H3" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="F3" s="3">
-        <v>42108.6348850162</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H3" s="3">
-        <v>42113.6348850164</v>
       </c>
       <c r="I3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="J3" s="3">
+      <c r="J3" s="5">
         <v>0</v>
       </c>
-      <c r="K3" s="3">
+      <c r="K3" s="5">
         <v>1000</v>
       </c>
-      <c r="L3" s="3">
+      <c r="L3" s="5">
         <v>0</v>
       </c>
-      <c r="M3" s="3">
+      <c r="M3" s="5">
         <v>1000</v>
       </c>
-      <c r="N3" s="3">
+      <c r="N3" s="5">
         <v>0</v>
       </c>
     </row>
@@ -603,34 +641,32 @@
       <c r="D4" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="3">
-        <v>42108.6348850165</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H4" s="3">
-        <v>42118.6348850166</v>
+      <c r="E4" s="3"/>
+      <c r="F4" s="4">
+        <v>42108.8494301613</v>
+      </c>
+      <c r="G4" s="4">
+        <v>42118.8494301614</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="J4" s="3">
+        <v>27</v>
+      </c>
+      <c r="J4" s="5">
         <v>0</v>
       </c>
-      <c r="K4" s="3">
+      <c r="K4" s="5">
         <v>10000</v>
       </c>
-      <c r="L4" s="3">
+      <c r="L4" s="5">
         <v>10</v>
       </c>
-      <c r="M4" s="3">
+      <c r="M4" s="5">
         <v>100</v>
       </c>
-      <c r="N4" s="3">
+      <c r="N4" s="5">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
finished writing/reading of resources, risk analysis and baseline schedule
</commit_message>
<xml_diff>
--- a/PMConverter/src/test.xlsx
+++ b/PMConverter/src/test.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="45">
   <si>
     <t>General</t>
   </si>
@@ -100,6 +100,57 @@
   </si>
   <si>
     <t>Tester [50.0 #]</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Availability</t>
+  </si>
+  <si>
+    <t>Cost/Use</t>
+  </si>
+  <si>
+    <t>Cost/Unit</t>
+  </si>
+  <si>
+    <t>Assigned To</t>
+  </si>
+  <si>
+    <t>Programmer</t>
+  </si>
+  <si>
+    <t>Renewable</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> #</t>
+  </si>
+  <si>
+    <t>1[10 #];</t>
+  </si>
+  <si>
+    <t>Tester</t>
+  </si>
+  <si>
+    <t>1[5 #];2[50 #];</t>
+  </si>
+  <si>
+    <t>Activity Duration Distribution Profiles</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Optimistic</t>
+  </si>
+  <si>
+    <t>Most Probable</t>
+  </si>
+  <si>
+    <t>Pessimistic</t>
+  </si>
+  <si>
+    <t>manual - absolute</t>
   </si>
 </sst>
 </file>
@@ -108,6 +159,12 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy H:MM"/>
+    <numFmt numFmtId="165" formatCode="#,##0.00 €"/>
+    <numFmt numFmtId="164" formatCode="mm/dd/yyyy H:MM"/>
+    <numFmt numFmtId="164" formatCode="mm/dd/yyyy H:MM"/>
+    <numFmt numFmtId="165" formatCode="#,##0.00 €"/>
+    <numFmt numFmtId="165" formatCode="#,##0.00 €"/>
+    <numFmt numFmtId="165" formatCode="#,##0.00 €"/>
     <numFmt numFmtId="165" formatCode="#,##0.00 €"/>
   </numFmts>
   <fonts count="3">
@@ -134,7 +191,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -156,6 +213,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00FFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF008000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD4D0C8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -187,7 +262,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -202,6 +277,30 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -601,10 +700,10 @@
         <v>20</v>
       </c>
       <c r="F3" s="4">
-        <v>42108.849430161</v>
+        <v>42113.8552930887</v>
       </c>
       <c r="G3" s="4">
-        <v>42113.8494301611</v>
+        <v>42118.8552930888</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>21</v>
@@ -629,44 +728,44 @@
       </c>
     </row>
     <row r="4" spans="1:14">
-      <c r="A4" s="2">
+      <c r="A4" s="6">
         <v>2</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="3"/>
-      <c r="F4" s="4">
-        <v>42108.8494301613</v>
-      </c>
-      <c r="G4" s="4">
-        <v>42118.8494301614</v>
-      </c>
-      <c r="H4" s="3" t="s">
+      <c r="E4" s="6"/>
+      <c r="F4" s="8">
+        <v>42113.8552930891</v>
+      </c>
+      <c r="G4" s="9">
+        <v>42123.8552930891</v>
+      </c>
+      <c r="H4" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="I4" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="J4" s="5">
+      <c r="J4" s="10">
         <v>0</v>
       </c>
-      <c r="K4" s="5">
+      <c r="K4" s="11">
         <v>10000</v>
       </c>
-      <c r="L4" s="5">
+      <c r="L4" s="12">
         <v>10</v>
       </c>
-      <c r="M4" s="5">
+      <c r="M4" s="11">
         <v>100</v>
       </c>
-      <c r="N4" s="5">
+      <c r="N4" s="10">
         <v>0</v>
       </c>
     </row>
@@ -684,24 +783,214 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="1:8" ht="25" customHeight="1">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" s="13">
+        <v>0</v>
+      </c>
+      <c r="F3" s="13">
+        <v>100</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H3" s="5">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="2">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="13">
+        <v>0</v>
+      </c>
+      <c r="F4" s="13">
+        <v>75</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H4" s="5">
+        <v>315000</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="3.7109375" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" customWidth="1"/>
+    <col min="5" max="7" width="12.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="7">
+        <v>2</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E4" s="2">
+        <v>402</v>
+      </c>
+      <c r="F4" s="2">
+        <v>480</v>
+      </c>
+      <c r="G4" s="2">
+        <v>812</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:G1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>